<commit_message>
Adaptació data auxiliar per 2019
</commit_message>
<xml_diff>
--- a/data/Auxiliar_data/COBATEST_2019_Column_Mappings.xlsx
+++ b/data/Auxiliar_data/COBATEST_2019_Column_Mappings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER-PC\Desktop\GAD_CEEISCAT\COBATEST_Indicadors_2019\Data\Auxiliar_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER-PC\Desktop\GAD_CEEISCAT\COBATEST_2019\data\Auxiliar_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5393DA2-EBB6-4844-8B50-E1EE11ADE4FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA307EC6-AAEA-4AC4-BCF9-2CC0C9B3F2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="137">
   <si>
     <t>COBATEST_Variable_name</t>
   </si>
@@ -259,9 +259,6 @@
     <t>Exaequo</t>
   </si>
   <si>
-    <t>Violett</t>
-  </si>
-  <si>
     <t>Adhara 2019 clean.dta</t>
   </si>
   <si>
@@ -280,9 +277,6 @@
     <t>ScreeningHIVtestResult</t>
   </si>
   <si>
-    <t>DDBB_stata_final</t>
-  </si>
-  <si>
     <t>centre</t>
   </si>
   <si>
@@ -428,6 +422,21 @@
   </si>
   <si>
     <t>ResultLastHIV</t>
+  </si>
+  <si>
+    <t>COBATEST_EspacePBELGIUM_2019.xlsx</t>
+  </si>
+  <si>
+    <t>Finaal_Cobatest_document_Violett_proc.xlsx</t>
+  </si>
+  <si>
+    <t>SyphScreeningTest</t>
+  </si>
+  <si>
+    <t>HCVScreeningTest</t>
+  </si>
+  <si>
+    <t>COBATEST 2019 clean data for indicators_20230427.dta</t>
   </si>
 </sst>
 </file>
@@ -546,24 +555,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -845,98 +847,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.9375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.9296875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="37.1171875" style="11" customWidth="1"/>
-    <col min="2" max="3" width="27.46875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.3515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.46875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5859375" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.1171875" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.8203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.76171875" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.8203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="27.3515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.9375" style="11"/>
+    <col min="1" max="1" width="37.1328125" customWidth="1"/>
+    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.9296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="17" t="s">
+      <c r="B1" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="17" t="s">
+      <c r="L1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -947,11 +951,11 @@
         <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+        <v>117</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
         <v>19</v>
       </c>
@@ -964,7 +968,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -975,15 +979,15 @@
         <v>18</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8" t="s">
-        <v>110</v>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>2</v>
@@ -992,68 +996,70 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="C5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
+        <v>94</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1062,37 +1068,36 @@
       <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="12"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -1110,32 +1115,31 @@
       <c r="H8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="L8" s="8" t="s">
+      <c r="J8" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M8" s="12"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>22</v>
@@ -1149,32 +1153,31 @@
       <c r="H9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="K9" s="8" t="s">
+      <c r="J9" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="L9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="12"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>23</v>
@@ -1188,28 +1191,27 @@
       <c r="H10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="K10" s="8" t="s">
+      <c r="J10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="M10" s="12"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="L10" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -1225,28 +1227,27 @@
       <c r="H11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="L11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M11" s="12"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -1262,28 +1263,27 @@
       <c r="H12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M12" s="12"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -1299,10 +1299,10 @@
       <c r="H13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="4" t="s">
         <v>26</v>
       </c>
       <c r="K13" s="4" t="s">
@@ -1312,14 +1312,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -1335,10 +1335,10 @@
       <c r="H14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="4" t="s">
         <v>27</v>
       </c>
       <c r="K14" s="4" t="s">
@@ -1348,23 +1348,23 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" s="9" t="s">
+      <c r="D15" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G15" s="4" t="s">
@@ -1373,11 +1373,11 @@
       <c r="H15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>114</v>
+      <c r="J15" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>1</v>
@@ -1386,14 +1386,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -1406,16 +1406,16 @@
         <v>28</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>115</v>
+      <c r="J16" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>10</v>
@@ -1424,34 +1424,32 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="6"/>
+        <v>131</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
       <c r="K17" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -1469,11 +1467,11 @@
       <c r="H18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J18" s="8" t="s">
-        <v>116</v>
+      <c r="J18" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>11</v>
@@ -1482,14 +1480,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -1498,20 +1496,20 @@
       <c r="E19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="H19" s="8" t="s">
+      <c r="G19" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J19" s="8" t="s">
-        <v>117</v>
+      <c r="J19" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>12</v>
@@ -1520,71 +1518,71 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
+        <v>95</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H21" s="8" t="s">
+      <c r="G21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" s="4" t="s">
         <v>31</v>
       </c>
       <c r="K21" s="4" t="s">
@@ -1594,14 +1592,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="4" t="s">
@@ -1610,19 +1608,19 @@
       <c r="E22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="H22" s="8" t="s">
+      <c r="G22" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="4" t="s">
         <v>32</v>
       </c>
       <c r="K22" s="4" t="s">
@@ -1632,139 +1630,139 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>98</v>
+      <c r="H23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A24" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A25" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="B25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="D26" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6" t="s">
+      <c r="G26" s="4"/>
+      <c r="H26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8" t="s">
+      <c r="I26" s="4"/>
+      <c r="J26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="K26" s="4"/>
@@ -1772,825 +1770,849 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6" t="s">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6" t="s">
+      <c r="G27" s="4"/>
+      <c r="H27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8" t="s">
+      <c r="I27" s="4"/>
+      <c r="J27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8" t="s">
+      <c r="K27" s="4"/>
+      <c r="L27" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6" t="s">
+      <c r="G28" s="4"/>
+      <c r="H28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8" t="s">
+      <c r="I28" s="4"/>
+      <c r="J28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8" t="s">
+      <c r="K28" s="4"/>
+      <c r="L28" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="K29" s="8"/>
+        <v>99</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K29" s="4"/>
       <c r="L29" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
+        <v>100</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6" t="s">
+      <c r="G31" s="4"/>
+      <c r="H31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8" t="s">
+      <c r="I31" s="4"/>
+      <c r="J31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8" t="s">
+      <c r="K31" s="4"/>
+      <c r="L31" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D32" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="F32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E33" s="6" t="s">
+      <c r="D33" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6" t="s">
+      <c r="G33" s="4"/>
+      <c r="H33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8" t="s">
+      <c r="I33" s="4"/>
+      <c r="J33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8" t="s">
+      <c r="K33" s="4"/>
+      <c r="L33" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6" t="s">
+      <c r="G34" s="4"/>
+      <c r="H34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8" t="s">
+      <c r="I34" s="4"/>
+      <c r="J34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8" t="s">
+      <c r="K34" s="4"/>
+      <c r="L34" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A35" s="14" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8" t="s">
+      <c r="E35" s="4"/>
+      <c r="F35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8" t="s">
+      <c r="K35" s="4"/>
+      <c r="L35" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A36" s="14" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A37" s="14" t="s">
+      <c r="H37" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9" t="s">
+      <c r="I37" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="J37" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G37" s="8" t="s">
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A40" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A42" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A43" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G43" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H37" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A38" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A39" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G39" s="8" t="s">
+      <c r="H43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A44" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A45" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A46" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G46" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H39" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I39" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A40" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I40" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A41" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A42" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G42" s="8" t="s">
+      <c r="H46" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A47" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G47" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H42" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A43" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="J43" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="K43" s="9"/>
-      <c r="L43" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A44" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H44" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I44" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J44" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A45" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G45" s="8" t="s">
+      <c r="H47" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G48" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H45" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I45" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A46" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H46" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I46" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A47" s="14" t="s">
+      <c r="H48" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9" t="s">
+      <c r="I48" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="J48" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J47" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A48" s="14" t="s">
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A49" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A50" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B50" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C50" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D50" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8" t="s">
+      <c r="E50" s="4"/>
+      <c r="F50" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="G50" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H48" s="8" t="s">
+      <c r="H50" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="I50" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J48" s="8" t="s">
+      <c r="J50" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8" t="s">
+      <c r="K50" s="4"/>
+      <c r="L50" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A49" s="14" t="s">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A51" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B51" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C51" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D51" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8" t="s">
+      <c r="E51" s="4"/>
+      <c r="F51" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8" t="s">
+      <c r="G51" s="4"/>
+      <c r="H51" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8" t="s">
+      <c r="I51" s="4"/>
+      <c r="J51" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8" t="s">
+      <c r="K51" s="4"/>
+      <c r="L51" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A50" s="14" t="s">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A52" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B52" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C52" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D52" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8" t="s">
+      <c r="E52" s="4"/>
+      <c r="F52" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8" t="s">
+      <c r="G52" s="4"/>
+      <c r="H52" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8" t="s">
+      <c r="I52" s="4"/>
+      <c r="J52" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8" t="s">
+      <c r="K52" s="4"/>
+      <c r="L52" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A51" s="15" t="s">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A53" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B53" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C53" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D53" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10" t="s">
+      <c r="E53" s="7"/>
+      <c r="F53" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G51" s="10" t="s">
+      <c r="G53" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H51" s="10" t="s">
+      <c r="H53" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I51" s="10" t="s">
+      <c r="I53" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J51" s="10" t="s">
+      <c r="J53" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K51" s="10"/>
-      <c r="L51" s="10" t="s">
+      <c r="K53" s="7"/>
+      <c r="L53" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="12"/>
-      <c r="K52" s="12"/>
-      <c r="L52" s="12"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="K54" s="12"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A55" s="13"/>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A57" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2606,13 +2628,13 @@
       <selection activeCell="C11" sqref="C11:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.17578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -2620,7 +2642,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2628,7 +2650,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2636,7 +2658,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -2644,7 +2666,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -2652,7 +2674,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -2660,7 +2682,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -2668,7 +2690,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -2676,7 +2698,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>74</v>
       </c>
@@ -2684,7 +2706,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -2692,20 +2714,20 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
         <v>79</v>
-      </c>
-      <c r="B11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
-      <c r="A12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>